<commit_message>
Organizar que el feature este todo alineado
</commit_message>
<xml_diff>
--- a/Documentos/Plan Qa.xlsx
+++ b/Documentos/Plan Qa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9225" tabRatio="544"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9225" tabRatio="544" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de Pruebas GUIA-NoOficial" sheetId="1" r:id="rId1"/>
@@ -2464,6 +2464,300 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2493,310 +2787,16 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2853,7 +2853,7 @@
         <xdr:cNvPr id="7" name="1 Grupo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2872,7 +2872,7 @@
           <xdr:cNvPr id="8" name="2 Triángulo isósceles">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2916,7 +2916,7 @@
           <xdr:cNvPr id="9" name="3 CuadroTexto">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2968,7 +2968,7 @@
           <xdr:cNvPr id="10" name="4 CuadroTexto">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3019,7 +3019,7 @@
           <xdr:cNvPr id="11" name="5 CuadroTexto">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3088,7 +3088,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3156,7 +3156,7 @@
         <xdr:cNvPr id="2" name="Flecha: a la derecha 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F11EFA6-F96F-4D3C-A0D7-86F7F846B3A8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F11EFA6-F96F-4D3C-A0D7-86F7F846B3A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3223,7 +3223,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3869,7 +3869,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3879,7 +3879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A92" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A74" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <selection activeCell="C6" sqref="C6:I6"/>
     </sheetView>
   </sheetViews>
@@ -3898,158 +3898,158 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1">
-      <c r="B1" s="153"/>
-      <c r="C1" s="153"/>
-      <c r="D1" s="153"/>
-      <c r="E1" s="153"/>
-      <c r="F1" s="153"/>
-      <c r="G1" s="153"/>
-      <c r="H1" s="153"/>
-      <c r="I1" s="153"/>
+      <c r="B1" s="165"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="165"/>
+      <c r="E1" s="165"/>
+      <c r="F1" s="165"/>
+      <c r="G1" s="165"/>
+      <c r="H1" s="165"/>
+      <c r="I1" s="165"/>
     </row>
     <row r="2" spans="2:9" ht="39" customHeight="1" thickBot="1">
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="186" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="155"/>
-      <c r="H2" s="155"/>
-      <c r="I2" s="156"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="188"/>
     </row>
     <row r="3" spans="2:9" ht="7.5" customHeight="1">
-      <c r="B3" s="153"/>
-      <c r="C3" s="153"/>
-      <c r="D3" s="153"/>
-      <c r="E3" s="153"/>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="153"/>
-      <c r="I3" s="153"/>
+      <c r="B3" s="165"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="165"/>
+      <c r="E3" s="165"/>
+      <c r="F3" s="165"/>
+      <c r="G3" s="165"/>
+      <c r="H3" s="165"/>
+      <c r="I3" s="165"/>
     </row>
     <row r="4" spans="2:9" ht="7.5" customHeight="1" thickBot="1">
-      <c r="B4" s="153"/>
-      <c r="C4" s="153"/>
-      <c r="D4" s="153"/>
-      <c r="E4" s="153"/>
-      <c r="F4" s="153"/>
-      <c r="G4" s="153"/>
-      <c r="H4" s="153"/>
-      <c r="I4" s="153"/>
+      <c r="B4" s="165"/>
+      <c r="C4" s="165"/>
+      <c r="D4" s="165"/>
+      <c r="E4" s="165"/>
+      <c r="F4" s="165"/>
+      <c r="G4" s="165"/>
+      <c r="H4" s="165"/>
+      <c r="I4" s="165"/>
     </row>
     <row r="5" spans="2:9" ht="15">
-      <c r="B5" s="159" t="s">
+      <c r="B5" s="189" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="160"/>
-      <c r="D5" s="160"/>
-      <c r="E5" s="160"/>
-      <c r="F5" s="160"/>
-      <c r="G5" s="160"/>
-      <c r="H5" s="160"/>
-      <c r="I5" s="161"/>
+      <c r="C5" s="190"/>
+      <c r="D5" s="190"/>
+      <c r="E5" s="190"/>
+      <c r="F5" s="190"/>
+      <c r="G5" s="190"/>
+      <c r="H5" s="190"/>
+      <c r="I5" s="191"/>
     </row>
     <row r="6" spans="2:9" ht="15">
       <c r="B6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="182" t="s">
         <v>202</v>
       </c>
-      <c r="D6" s="157"/>
-      <c r="E6" s="157"/>
-      <c r="F6" s="157"/>
-      <c r="G6" s="157"/>
-      <c r="H6" s="157"/>
-      <c r="I6" s="158"/>
+      <c r="D6" s="182"/>
+      <c r="E6" s="182"/>
+      <c r="F6" s="182"/>
+      <c r="G6" s="182"/>
+      <c r="H6" s="182"/>
+      <c r="I6" s="183"/>
     </row>
     <row r="7" spans="2:9" ht="15">
       <c r="B7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="157" t="s">
+      <c r="C7" s="182" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="157"/>
-      <c r="E7" s="157"/>
-      <c r="F7" s="157"/>
-      <c r="G7" s="157"/>
-      <c r="H7" s="157"/>
-      <c r="I7" s="158"/>
+      <c r="D7" s="182"/>
+      <c r="E7" s="182"/>
+      <c r="F7" s="182"/>
+      <c r="G7" s="182"/>
+      <c r="H7" s="182"/>
+      <c r="I7" s="183"/>
     </row>
     <row r="8" spans="2:9" ht="15">
-      <c r="B8" s="179" t="s">
+      <c r="B8" s="174" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="157" t="s">
+      <c r="D8" s="182" t="s">
         <v>203</v>
       </c>
-      <c r="E8" s="157"/>
-      <c r="F8" s="157"/>
-      <c r="G8" s="157"/>
-      <c r="H8" s="157"/>
-      <c r="I8" s="158"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="182"/>
+      <c r="G8" s="182"/>
+      <c r="H8" s="182"/>
+      <c r="I8" s="183"/>
     </row>
     <row r="9" spans="2:9" ht="15">
-      <c r="B9" s="179"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="157" t="s">
+      <c r="D9" s="182" t="s">
         <v>180</v>
       </c>
-      <c r="E9" s="157"/>
-      <c r="F9" s="157"/>
-      <c r="G9" s="157"/>
-      <c r="H9" s="157"/>
-      <c r="I9" s="158"/>
+      <c r="E9" s="182"/>
+      <c r="F9" s="182"/>
+      <c r="G9" s="182"/>
+      <c r="H9" s="182"/>
+      <c r="I9" s="183"/>
     </row>
     <row r="10" spans="2:9" ht="15">
-      <c r="B10" s="179"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="176" t="s">
+      <c r="D10" s="184" t="s">
         <v>222</v>
       </c>
-      <c r="E10" s="157"/>
-      <c r="F10" s="157"/>
-      <c r="G10" s="157"/>
-      <c r="H10" s="157"/>
-      <c r="I10" s="158"/>
+      <c r="E10" s="182"/>
+      <c r="F10" s="182"/>
+      <c r="G10" s="182"/>
+      <c r="H10" s="182"/>
+      <c r="I10" s="183"/>
     </row>
     <row r="11" spans="2:9" ht="15">
       <c r="B11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="157" t="s">
+      <c r="C11" s="182" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="157"/>
-      <c r="E11" s="157"/>
-      <c r="F11" s="157"/>
-      <c r="G11" s="157"/>
-      <c r="H11" s="157"/>
-      <c r="I11" s="158"/>
+      <c r="D11" s="182"/>
+      <c r="E11" s="182"/>
+      <c r="F11" s="182"/>
+      <c r="G11" s="182"/>
+      <c r="H11" s="182"/>
+      <c r="I11" s="183"/>
     </row>
     <row r="12" spans="2:9" ht="30.75" thickBot="1">
       <c r="B12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="162" t="s">
+      <c r="C12" s="192" t="s">
         <v>204</v>
       </c>
-      <c r="D12" s="163"/>
-      <c r="E12" s="163"/>
-      <c r="F12" s="163"/>
-      <c r="G12" s="163"/>
-      <c r="H12" s="163"/>
-      <c r="I12" s="164"/>
+      <c r="D12" s="193"/>
+      <c r="E12" s="193"/>
+      <c r="F12" s="193"/>
+      <c r="G12" s="193"/>
+      <c r="H12" s="193"/>
+      <c r="I12" s="194"/>
     </row>
     <row r="13" spans="2:9" ht="15" thickBot="1"/>
     <row r="14" spans="2:9" ht="15">
@@ -4065,76 +4065,76 @@
       <c r="I14" s="18"/>
     </row>
     <row r="15" spans="2:9">
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="195" t="s">
         <v>205</v>
       </c>
-      <c r="C15" s="134"/>
-      <c r="D15" s="134"/>
-      <c r="E15" s="134"/>
-      <c r="F15" s="134"/>
-      <c r="G15" s="134"/>
-      <c r="H15" s="134"/>
-      <c r="I15" s="166"/>
+      <c r="C15" s="135"/>
+      <c r="D15" s="135"/>
+      <c r="E15" s="135"/>
+      <c r="F15" s="135"/>
+      <c r="G15" s="135"/>
+      <c r="H15" s="135"/>
+      <c r="I15" s="196"/>
     </row>
     <row r="16" spans="2:9">
-      <c r="B16" s="165"/>
-      <c r="C16" s="134"/>
-      <c r="D16" s="134"/>
-      <c r="E16" s="134"/>
-      <c r="F16" s="134"/>
-      <c r="G16" s="134"/>
-      <c r="H16" s="134"/>
-      <c r="I16" s="166"/>
+      <c r="B16" s="195"/>
+      <c r="C16" s="135"/>
+      <c r="D16" s="135"/>
+      <c r="E16" s="135"/>
+      <c r="F16" s="135"/>
+      <c r="G16" s="135"/>
+      <c r="H16" s="135"/>
+      <c r="I16" s="196"/>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="165"/>
-      <c r="C17" s="134"/>
-      <c r="D17" s="134"/>
-      <c r="E17" s="134"/>
-      <c r="F17" s="134"/>
-      <c r="G17" s="134"/>
-      <c r="H17" s="134"/>
-      <c r="I17" s="166"/>
+      <c r="B17" s="195"/>
+      <c r="C17" s="135"/>
+      <c r="D17" s="135"/>
+      <c r="E17" s="135"/>
+      <c r="F17" s="135"/>
+      <c r="G17" s="135"/>
+      <c r="H17" s="135"/>
+      <c r="I17" s="196"/>
     </row>
     <row r="18" spans="2:9">
-      <c r="B18" s="165"/>
-      <c r="C18" s="134"/>
-      <c r="D18" s="134"/>
-      <c r="E18" s="134"/>
-      <c r="F18" s="134"/>
-      <c r="G18" s="134"/>
-      <c r="H18" s="134"/>
-      <c r="I18" s="166"/>
+      <c r="B18" s="195"/>
+      <c r="C18" s="135"/>
+      <c r="D18" s="135"/>
+      <c r="E18" s="135"/>
+      <c r="F18" s="135"/>
+      <c r="G18" s="135"/>
+      <c r="H18" s="135"/>
+      <c r="I18" s="196"/>
     </row>
     <row r="19" spans="2:9">
-      <c r="B19" s="165"/>
-      <c r="C19" s="134"/>
-      <c r="D19" s="134"/>
-      <c r="E19" s="134"/>
-      <c r="F19" s="134"/>
-      <c r="G19" s="134"/>
-      <c r="H19" s="134"/>
-      <c r="I19" s="166"/>
+      <c r="B19" s="195"/>
+      <c r="C19" s="135"/>
+      <c r="D19" s="135"/>
+      <c r="E19" s="135"/>
+      <c r="F19" s="135"/>
+      <c r="G19" s="135"/>
+      <c r="H19" s="135"/>
+      <c r="I19" s="196"/>
     </row>
     <row r="20" spans="2:9">
-      <c r="B20" s="165"/>
-      <c r="C20" s="134"/>
-      <c r="D20" s="134"/>
-      <c r="E20" s="134"/>
-      <c r="F20" s="134"/>
-      <c r="G20" s="134"/>
-      <c r="H20" s="134"/>
-      <c r="I20" s="166"/>
+      <c r="B20" s="195"/>
+      <c r="C20" s="135"/>
+      <c r="D20" s="135"/>
+      <c r="E20" s="135"/>
+      <c r="F20" s="135"/>
+      <c r="G20" s="135"/>
+      <c r="H20" s="135"/>
+      <c r="I20" s="196"/>
     </row>
     <row r="21" spans="2:9" ht="59.25" customHeight="1">
-      <c r="B21" s="131"/>
-      <c r="C21" s="132"/>
-      <c r="D21" s="132"/>
-      <c r="E21" s="132"/>
-      <c r="F21" s="132"/>
-      <c r="G21" s="132"/>
-      <c r="H21" s="132"/>
-      <c r="I21" s="167"/>
+      <c r="B21" s="197"/>
+      <c r="C21" s="198"/>
+      <c r="D21" s="198"/>
+      <c r="E21" s="198"/>
+      <c r="F21" s="198"/>
+      <c r="G21" s="198"/>
+      <c r="H21" s="198"/>
+      <c r="I21" s="199"/>
     </row>
     <row r="22" spans="2:9" ht="15" thickBot="1">
       <c r="B22" s="19"/>
@@ -4147,54 +4147,54 @@
       <c r="I22" s="19"/>
     </row>
     <row r="23" spans="2:9" ht="15">
-      <c r="B23" s="168" t="s">
+      <c r="B23" s="200" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="169"/>
-      <c r="D23" s="169"/>
-      <c r="E23" s="169"/>
-      <c r="F23" s="169"/>
-      <c r="G23" s="169"/>
-      <c r="H23" s="169"/>
-      <c r="I23" s="170"/>
+      <c r="C23" s="201"/>
+      <c r="D23" s="201"/>
+      <c r="E23" s="201"/>
+      <c r="F23" s="201"/>
+      <c r="G23" s="201"/>
+      <c r="H23" s="201"/>
+      <c r="I23" s="202"/>
     </row>
     <row r="24" spans="2:9" ht="15">
-      <c r="B24" s="137" t="s">
+      <c r="B24" s="215" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="138"/>
-      <c r="D24" s="138"/>
-      <c r="E24" s="138"/>
-      <c r="F24" s="139" t="s">
+      <c r="C24" s="216"/>
+      <c r="D24" s="216"/>
+      <c r="E24" s="216"/>
+      <c r="F24" s="217" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="139"/>
-      <c r="H24" s="139"/>
+      <c r="G24" s="217"/>
+      <c r="H24" s="217"/>
       <c r="I24" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="23.25" customHeight="1">
-      <c r="B25" s="171" t="s">
+      <c r="B25" s="203" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="172"/>
-      <c r="D25" s="172"/>
-      <c r="E25" s="172"/>
-      <c r="F25" s="172"/>
-      <c r="G25" s="172"/>
-      <c r="H25" s="172"/>
-      <c r="I25" s="173"/>
+      <c r="C25" s="204"/>
+      <c r="D25" s="204"/>
+      <c r="E25" s="204"/>
+      <c r="F25" s="204"/>
+      <c r="G25" s="204"/>
+      <c r="H25" s="204"/>
+      <c r="I25" s="205"/>
     </row>
     <row r="26" spans="2:9" ht="15">
-      <c r="B26" s="145" t="s">
+      <c r="B26" s="206" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="146"/>
-      <c r="D26" s="146" t="s">
+      <c r="C26" s="207"/>
+      <c r="D26" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="146"/>
+      <c r="E26" s="207"/>
       <c r="F26" s="20" t="s">
         <v>18</v>
       </c>
@@ -4209,14 +4209,14 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="60.75" customHeight="1">
-      <c r="B27" s="140" t="s">
+      <c r="B27" s="123" t="s">
         <v>165</v>
       </c>
-      <c r="C27" s="140"/>
-      <c r="D27" s="140" t="s">
+      <c r="C27" s="123"/>
+      <c r="D27" s="123" t="s">
         <v>206</v>
       </c>
-      <c r="E27" s="140"/>
+      <c r="E27" s="123"/>
       <c r="F27" s="99">
         <v>3</v>
       </c>
@@ -4232,14 +4232,14 @@
       </c>
     </row>
     <row r="28" spans="2:9" ht="75" customHeight="1">
-      <c r="B28" s="140" t="s">
+      <c r="B28" s="123" t="s">
         <v>166</v>
       </c>
-      <c r="C28" s="140"/>
-      <c r="D28" s="140" t="s">
+      <c r="C28" s="123"/>
+      <c r="D28" s="123" t="s">
         <v>207</v>
       </c>
-      <c r="E28" s="175"/>
+      <c r="E28" s="181"/>
       <c r="F28" s="99">
         <v>3</v>
       </c>
@@ -4255,14 +4255,14 @@
       </c>
     </row>
     <row r="29" spans="2:9" ht="60" customHeight="1">
-      <c r="B29" s="141" t="s">
+      <c r="B29" s="121" t="s">
         <v>167</v>
       </c>
-      <c r="C29" s="174"/>
-      <c r="D29" s="140" t="s">
+      <c r="C29" s="122"/>
+      <c r="D29" s="123" t="s">
         <v>208</v>
       </c>
-      <c r="E29" s="140"/>
+      <c r="E29" s="123"/>
       <c r="F29" s="99">
         <v>3</v>
       </c>
@@ -4278,14 +4278,14 @@
       </c>
     </row>
     <row r="30" spans="2:9" ht="66" customHeight="1">
-      <c r="B30" s="147" t="s">
+      <c r="B30" s="208" t="s">
         <v>168</v>
       </c>
-      <c r="C30" s="147"/>
-      <c r="D30" s="140" t="s">
+      <c r="C30" s="208"/>
+      <c r="D30" s="123" t="s">
         <v>209</v>
       </c>
-      <c r="E30" s="140"/>
+      <c r="E30" s="123"/>
       <c r="F30" s="99">
         <v>3</v>
       </c>
@@ -4301,14 +4301,14 @@
       </c>
     </row>
     <row r="31" spans="2:9" ht="63" customHeight="1">
-      <c r="B31" s="140" t="s">
+      <c r="B31" s="123" t="s">
         <v>210</v>
       </c>
-      <c r="C31" s="140"/>
-      <c r="D31" s="141" t="s">
+      <c r="C31" s="123"/>
+      <c r="D31" s="121" t="s">
         <v>211</v>
       </c>
-      <c r="E31" s="142"/>
+      <c r="E31" s="218"/>
       <c r="F31" s="99">
         <v>3</v>
       </c>
@@ -4324,14 +4324,14 @@
       </c>
     </row>
     <row r="32" spans="2:9" ht="41.25" customHeight="1">
-      <c r="B32" s="140" t="s">
+      <c r="B32" s="123" t="s">
         <v>170</v>
       </c>
-      <c r="C32" s="140"/>
-      <c r="D32" s="141" t="s">
+      <c r="C32" s="123"/>
+      <c r="D32" s="121" t="s">
         <v>171</v>
       </c>
-      <c r="E32" s="174"/>
+      <c r="E32" s="122"/>
       <c r="F32" s="99">
         <v>3</v>
       </c>
@@ -4347,14 +4347,14 @@
       </c>
     </row>
     <row r="33" spans="2:9" ht="43.5" customHeight="1">
-      <c r="B33" s="140" t="s">
+      <c r="B33" s="123" t="s">
         <v>169</v>
       </c>
-      <c r="C33" s="140"/>
-      <c r="D33" s="141" t="s">
+      <c r="C33" s="123"/>
+      <c r="D33" s="121" t="s">
         <v>212</v>
       </c>
-      <c r="E33" s="174"/>
+      <c r="E33" s="122"/>
       <c r="F33" s="99">
         <v>3</v>
       </c>
@@ -4380,10 +4380,10 @@
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="2:9">
-      <c r="B35" s="143"/>
-      <c r="C35" s="144"/>
-      <c r="D35" s="144"/>
-      <c r="E35" s="144"/>
+      <c r="B35" s="176"/>
+      <c r="C35" s="177"/>
+      <c r="D35" s="177"/>
+      <c r="E35" s="177"/>
       <c r="F35" s="25"/>
       <c r="G35" s="25"/>
       <c r="H35" s="25">
@@ -4393,26 +4393,26 @@
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="2:9" ht="19.5" customHeight="1">
-      <c r="B36" s="148" t="s">
+      <c r="B36" s="209" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="149"/>
-      <c r="D36" s="149"/>
-      <c r="E36" s="149"/>
-      <c r="F36" s="149"/>
-      <c r="G36" s="149"/>
-      <c r="H36" s="149"/>
-      <c r="I36" s="150"/>
+      <c r="C36" s="210"/>
+      <c r="D36" s="210"/>
+      <c r="E36" s="210"/>
+      <c r="F36" s="210"/>
+      <c r="G36" s="210"/>
+      <c r="H36" s="210"/>
+      <c r="I36" s="211"/>
     </row>
     <row r="37" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B37" s="145" t="s">
+      <c r="B37" s="206" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="146"/>
-      <c r="D37" s="146" t="s">
+      <c r="C37" s="207"/>
+      <c r="D37" s="207" t="s">
         <v>24</v>
       </c>
-      <c r="E37" s="146"/>
+      <c r="E37" s="207"/>
       <c r="F37" s="20" t="s">
         <v>18</v>
       </c>
@@ -4427,14 +4427,14 @@
       </c>
     </row>
     <row r="38" spans="2:9" s="3" customFormat="1" ht="30.75" customHeight="1">
-      <c r="B38" s="143" t="s">
+      <c r="B38" s="176" t="s">
         <v>213</v>
       </c>
-      <c r="C38" s="144"/>
-      <c r="D38" s="134" t="s">
+      <c r="C38" s="177"/>
+      <c r="D38" s="135" t="s">
         <v>182</v>
       </c>
-      <c r="E38" s="134"/>
+      <c r="E38" s="135"/>
       <c r="F38" s="25">
         <v>3</v>
       </c>
@@ -4453,10 +4453,10 @@
       <c r="B39" s="68" t="s">
         <v>214</v>
       </c>
-      <c r="D39" s="134" t="s">
+      <c r="D39" s="135" t="s">
         <v>182</v>
       </c>
-      <c r="E39" s="134"/>
+      <c r="E39" s="135"/>
       <c r="F39" s="67">
         <v>3</v>
       </c>
@@ -4475,10 +4475,10 @@
       <c r="B40" s="94" t="s">
         <v>215</v>
       </c>
-      <c r="D40" s="134" t="s">
+      <c r="D40" s="135" t="s">
         <v>182</v>
       </c>
-      <c r="E40" s="134"/>
+      <c r="E40" s="135"/>
       <c r="F40" s="92">
         <v>3</v>
       </c>
@@ -4494,10 +4494,10 @@
       </c>
     </row>
     <row r="41" spans="2:9" s="3" customFormat="1" ht="30.75" customHeight="1">
-      <c r="B41" s="143"/>
-      <c r="C41" s="144"/>
-      <c r="D41" s="134"/>
-      <c r="E41" s="134"/>
+      <c r="B41" s="176"/>
+      <c r="C41" s="177"/>
+      <c r="D41" s="135"/>
+      <c r="E41" s="135"/>
       <c r="F41" s="25"/>
       <c r="G41" s="25"/>
       <c r="H41" s="25">
@@ -4507,10 +4507,10 @@
       <c r="I41" s="4"/>
     </row>
     <row r="42" spans="2:9" s="3" customFormat="1" ht="30.75" customHeight="1">
-      <c r="B42" s="143"/>
-      <c r="C42" s="144"/>
-      <c r="D42" s="134"/>
-      <c r="E42" s="134"/>
+      <c r="B42" s="176"/>
+      <c r="C42" s="177"/>
+      <c r="D42" s="135"/>
+      <c r="E42" s="135"/>
       <c r="F42" s="25"/>
       <c r="G42" s="25"/>
       <c r="H42" s="25">
@@ -4520,10 +4520,10 @@
       <c r="I42" s="4"/>
     </row>
     <row r="43" spans="2:9" s="3" customFormat="1" ht="30.75" customHeight="1">
-      <c r="B43" s="143"/>
-      <c r="C43" s="144"/>
-      <c r="D43" s="134"/>
-      <c r="E43" s="134"/>
+      <c r="B43" s="176"/>
+      <c r="C43" s="177"/>
+      <c r="D43" s="135"/>
+      <c r="E43" s="135"/>
       <c r="F43" s="25"/>
       <c r="G43" s="25"/>
       <c r="H43" s="25">
@@ -4534,8 +4534,8 @@
     </row>
     <row r="44" spans="2:9" s="3" customFormat="1" ht="30.75" customHeight="1">
       <c r="B44" s="54"/>
-      <c r="D44" s="134"/>
-      <c r="E44" s="134"/>
+      <c r="D44" s="135"/>
+      <c r="E44" s="135"/>
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
       <c r="H44" s="25">
@@ -4546,8 +4546,8 @@
     </row>
     <row r="45" spans="2:9" s="3" customFormat="1" ht="30.75" customHeight="1">
       <c r="B45" s="97"/>
-      <c r="D45" s="134"/>
-      <c r="E45" s="134"/>
+      <c r="D45" s="135"/>
+      <c r="E45" s="135"/>
       <c r="F45" s="98"/>
       <c r="G45" s="25"/>
       <c r="H45" s="25">
@@ -4558,8 +4558,8 @@
     </row>
     <row r="46" spans="2:9" s="3" customFormat="1" ht="30.75" customHeight="1">
       <c r="B46" s="54"/>
-      <c r="D46" s="180"/>
-      <c r="E46" s="180"/>
+      <c r="D46" s="178"/>
+      <c r="E46" s="178"/>
       <c r="F46" s="25"/>
       <c r="G46" s="25"/>
       <c r="H46" s="25">
@@ -4569,10 +4569,10 @@
       <c r="I46" s="4"/>
     </row>
     <row r="47" spans="2:9" s="3" customFormat="1" ht="30.75" customHeight="1">
-      <c r="B47" s="143"/>
-      <c r="C47" s="144"/>
-      <c r="D47" s="180"/>
-      <c r="E47" s="180"/>
+      <c r="B47" s="176"/>
+      <c r="C47" s="177"/>
+      <c r="D47" s="178"/>
+      <c r="E47" s="178"/>
       <c r="F47" s="25"/>
       <c r="G47" s="25"/>
       <c r="H47" s="25">
@@ -4582,10 +4582,10 @@
       <c r="I47" s="4"/>
     </row>
     <row r="48" spans="2:9" s="3" customFormat="1" ht="30.75" customHeight="1">
-      <c r="B48" s="181"/>
-      <c r="C48" s="182"/>
-      <c r="D48" s="180"/>
-      <c r="E48" s="180"/>
+      <c r="B48" s="179"/>
+      <c r="C48" s="180"/>
+      <c r="D48" s="178"/>
+      <c r="E48" s="178"/>
       <c r="F48" s="25"/>
       <c r="G48" s="25"/>
       <c r="H48" s="25">
@@ -4595,10 +4595,10 @@
       <c r="I48" s="4"/>
     </row>
     <row r="49" spans="2:9" s="3" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B49" s="151"/>
-      <c r="C49" s="152"/>
-      <c r="D49" s="152"/>
-      <c r="E49" s="152"/>
+      <c r="B49" s="185"/>
+      <c r="C49" s="175"/>
+      <c r="D49" s="175"/>
+      <c r="E49" s="175"/>
       <c r="F49" s="11"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11">
@@ -4622,11 +4622,11 @@
     </row>
     <row r="52" spans="2:9" ht="21.75" customHeight="1">
       <c r="B52" s="9"/>
-      <c r="C52" s="133" t="s">
+      <c r="C52" s="212" t="s">
         <v>17</v>
       </c>
-      <c r="D52" s="133"/>
-      <c r="E52" s="133"/>
+      <c r="D52" s="212"/>
+      <c r="E52" s="212"/>
       <c r="F52" s="23" t="s">
         <v>27</v>
       </c>
@@ -4639,81 +4639,81 @@
       <c r="I52" s="10"/>
     </row>
     <row r="53" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B53" s="178" t="s">
+      <c r="B53" s="144" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="184" t="s">
+      <c r="C53" s="145" t="s">
         <v>217</v>
       </c>
-      <c r="D53" s="185"/>
-      <c r="E53" s="186"/>
-      <c r="F53" s="228"/>
-      <c r="G53" s="183" t="s">
+      <c r="D53" s="146"/>
+      <c r="E53" s="147"/>
+      <c r="F53" s="151"/>
+      <c r="G53" s="143" t="s">
         <v>93</v>
       </c>
-      <c r="H53" s="177"/>
+      <c r="H53" s="142"/>
       <c r="I53" s="10"/>
     </row>
     <row r="54" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B54" s="178"/>
-      <c r="C54" s="187"/>
-      <c r="D54" s="188"/>
-      <c r="E54" s="189"/>
-      <c r="F54" s="228"/>
-      <c r="G54" s="183"/>
-      <c r="H54" s="177"/>
+      <c r="B54" s="144"/>
+      <c r="C54" s="148"/>
+      <c r="D54" s="149"/>
+      <c r="E54" s="150"/>
+      <c r="F54" s="151"/>
+      <c r="G54" s="143"/>
+      <c r="H54" s="142"/>
       <c r="I54" s="10"/>
     </row>
     <row r="55" spans="2:9" ht="90.75" customHeight="1">
-      <c r="B55" s="178" t="s">
+      <c r="B55" s="144" t="s">
         <v>31</v>
       </c>
-      <c r="C55" s="184" t="s">
+      <c r="C55" s="145" t="s">
         <v>218</v>
       </c>
-      <c r="D55" s="185"/>
-      <c r="E55" s="186"/>
-      <c r="F55" s="177"/>
-      <c r="G55" s="183"/>
-      <c r="H55" s="177" t="s">
+      <c r="D55" s="146"/>
+      <c r="E55" s="147"/>
+      <c r="F55" s="142"/>
+      <c r="G55" s="143"/>
+      <c r="H55" s="142" t="s">
         <v>93</v>
       </c>
       <c r="I55" s="10"/>
     </row>
     <row r="56" spans="2:9" ht="33" customHeight="1">
-      <c r="B56" s="178"/>
-      <c r="C56" s="187"/>
-      <c r="D56" s="188"/>
-      <c r="E56" s="189"/>
-      <c r="F56" s="177"/>
-      <c r="G56" s="183"/>
-      <c r="H56" s="177"/>
+      <c r="B56" s="144"/>
+      <c r="C56" s="148"/>
+      <c r="D56" s="149"/>
+      <c r="E56" s="150"/>
+      <c r="F56" s="142"/>
+      <c r="G56" s="143"/>
+      <c r="H56" s="142"/>
       <c r="I56" s="10"/>
     </row>
     <row r="57" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B57" s="178" t="s">
+      <c r="B57" s="144" t="s">
         <v>32</v>
       </c>
-      <c r="C57" s="222" t="s">
+      <c r="C57" s="136" t="s">
         <v>219</v>
       </c>
-      <c r="D57" s="223"/>
-      <c r="E57" s="224"/>
-      <c r="F57" s="177" t="s">
+      <c r="D57" s="137"/>
+      <c r="E57" s="138"/>
+      <c r="F57" s="142" t="s">
         <v>93</v>
       </c>
-      <c r="G57" s="183"/>
-      <c r="H57" s="183"/>
+      <c r="G57" s="143"/>
+      <c r="H57" s="143"/>
       <c r="I57" s="10"/>
     </row>
     <row r="58" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B58" s="178"/>
-      <c r="C58" s="225"/>
-      <c r="D58" s="226"/>
-      <c r="E58" s="227"/>
-      <c r="F58" s="177"/>
-      <c r="G58" s="183"/>
-      <c r="H58" s="183"/>
+      <c r="B58" s="144"/>
+      <c r="C58" s="139"/>
+      <c r="D58" s="140"/>
+      <c r="E58" s="141"/>
+      <c r="F58" s="142"/>
+      <c r="G58" s="143"/>
+      <c r="H58" s="143"/>
       <c r="I58" s="10"/>
     </row>
     <row r="59" spans="2:9" ht="15.75" customHeight="1" thickBot="1">
@@ -4728,111 +4728,111 @@
     </row>
     <row r="60" spans="2:9" ht="15" thickBot="1"/>
     <row r="61" spans="2:9" ht="41.25" customHeight="1" thickBot="1">
-      <c r="B61" s="216" t="s">
+      <c r="B61" s="129" t="s">
         <v>33</v>
       </c>
-      <c r="C61" s="217"/>
-      <c r="D61" s="217"/>
-      <c r="E61" s="217"/>
-      <c r="F61" s="217"/>
-      <c r="G61" s="217"/>
-      <c r="H61" s="217"/>
-      <c r="I61" s="218"/>
+      <c r="C61" s="130"/>
+      <c r="D61" s="130"/>
+      <c r="E61" s="130"/>
+      <c r="F61" s="130"/>
+      <c r="G61" s="130"/>
+      <c r="H61" s="130"/>
+      <c r="I61" s="131"/>
     </row>
     <row r="62" spans="2:9" ht="41.25" customHeight="1" thickBot="1">
-      <c r="B62" s="124" t="s">
+      <c r="B62" s="222" t="s">
         <v>231</v>
       </c>
-      <c r="C62" s="125"/>
-      <c r="D62" s="125"/>
-      <c r="E62" s="125"/>
-      <c r="F62" s="125"/>
-      <c r="G62" s="125"/>
-      <c r="H62" s="125"/>
-      <c r="I62" s="126"/>
+      <c r="C62" s="223"/>
+      <c r="D62" s="223"/>
+      <c r="E62" s="223"/>
+      <c r="F62" s="223"/>
+      <c r="G62" s="223"/>
+      <c r="H62" s="223"/>
+      <c r="I62" s="224"/>
     </row>
     <row r="63" spans="2:9" ht="144.75" customHeight="1" thickBot="1">
       <c r="B63" s="116">
         <v>1</v>
       </c>
-      <c r="C63" s="127" t="s">
+      <c r="C63" s="225" t="s">
         <v>225</v>
       </c>
-      <c r="D63" s="128"/>
-      <c r="E63" s="128"/>
-      <c r="F63" s="128"/>
-      <c r="G63" s="128"/>
-      <c r="H63" s="129"/>
+      <c r="D63" s="226"/>
+      <c r="E63" s="226"/>
+      <c r="F63" s="226"/>
+      <c r="G63" s="226"/>
+      <c r="H63" s="227"/>
       <c r="I63" s="117"/>
     </row>
     <row r="64" spans="2:9" ht="101.25" customHeight="1" thickBot="1">
       <c r="B64" s="116">
         <v>2</v>
       </c>
-      <c r="C64" s="123" t="s">
+      <c r="C64" s="221" t="s">
         <v>226</v>
       </c>
-      <c r="D64" s="130"/>
-      <c r="E64" s="130"/>
-      <c r="F64" s="130"/>
-      <c r="G64" s="130"/>
-      <c r="H64" s="130"/>
+      <c r="D64" s="228"/>
+      <c r="E64" s="228"/>
+      <c r="F64" s="228"/>
+      <c r="G64" s="228"/>
+      <c r="H64" s="228"/>
       <c r="I64" s="69"/>
     </row>
     <row r="65" spans="2:9" ht="36" customHeight="1" thickBot="1">
       <c r="B65" s="116">
         <v>3</v>
       </c>
-      <c r="C65" s="123" t="s">
+      <c r="C65" s="221" t="s">
         <v>227</v>
       </c>
-      <c r="D65" s="130"/>
-      <c r="E65" s="130"/>
-      <c r="F65" s="130"/>
-      <c r="G65" s="130"/>
-      <c r="H65" s="130"/>
+      <c r="D65" s="228"/>
+      <c r="E65" s="228"/>
+      <c r="F65" s="228"/>
+      <c r="G65" s="228"/>
+      <c r="H65" s="228"/>
       <c r="I65" s="110"/>
     </row>
     <row r="66" spans="2:9" ht="97.5" customHeight="1" thickBot="1">
       <c r="B66" s="116">
         <v>4</v>
       </c>
-      <c r="C66" s="123" t="s">
+      <c r="C66" s="221" t="s">
         <v>228</v>
       </c>
-      <c r="D66" s="130"/>
-      <c r="E66" s="130"/>
-      <c r="F66" s="130"/>
-      <c r="G66" s="130"/>
-      <c r="H66" s="130"/>
+      <c r="D66" s="228"/>
+      <c r="E66" s="228"/>
+      <c r="F66" s="228"/>
+      <c r="G66" s="228"/>
+      <c r="H66" s="228"/>
       <c r="I66" s="110"/>
     </row>
     <row r="67" spans="2:9" ht="35.25" customHeight="1" thickBot="1">
       <c r="B67" s="120">
         <v>5</v>
       </c>
-      <c r="C67" s="130" t="s">
+      <c r="C67" s="228" t="s">
         <v>229</v>
       </c>
-      <c r="D67" s="130"/>
-      <c r="E67" s="130"/>
-      <c r="F67" s="130"/>
-      <c r="G67" s="130"/>
-      <c r="H67" s="130"/>
+      <c r="D67" s="228"/>
+      <c r="E67" s="228"/>
+      <c r="F67" s="228"/>
+      <c r="G67" s="228"/>
+      <c r="H67" s="228"/>
       <c r="I67" s="110"/>
     </row>
     <row r="68" spans="2:9" ht="43.5" customHeight="1" thickBot="1">
       <c r="B68" s="120">
         <v>6</v>
       </c>
-      <c r="C68" s="121" t="s">
+      <c r="C68" s="219" t="s">
         <v>230</v>
       </c>
-      <c r="D68" s="122"/>
-      <c r="E68" s="122"/>
-      <c r="F68" s="122"/>
-      <c r="G68" s="122"/>
-      <c r="H68" s="123"/>
+      <c r="D68" s="220"/>
+      <c r="E68" s="220"/>
+      <c r="F68" s="220"/>
+      <c r="G68" s="220"/>
+      <c r="H68" s="221"/>
       <c r="I68" s="110"/>
     </row>
     <row r="69" spans="2:9" ht="100.5" customHeight="1" thickBot="1">
@@ -4846,72 +4846,72 @@
       <c r="I69" s="112"/>
     </row>
     <row r="70" spans="2:9" ht="29.25" customHeight="1">
-      <c r="B70" s="219" t="s">
+      <c r="B70" s="132" t="s">
         <v>34</v>
       </c>
-      <c r="C70" s="220"/>
-      <c r="D70" s="220"/>
-      <c r="E70" s="220"/>
-      <c r="F70" s="220"/>
-      <c r="G70" s="220"/>
-      <c r="H70" s="220"/>
-      <c r="I70" s="221"/>
+      <c r="C70" s="133"/>
+      <c r="D70" s="133"/>
+      <c r="E70" s="133"/>
+      <c r="F70" s="133"/>
+      <c r="G70" s="133"/>
+      <c r="H70" s="133"/>
+      <c r="I70" s="134"/>
     </row>
     <row r="71" spans="2:9">
-      <c r="B71" s="202" t="s">
+      <c r="B71" s="124" t="s">
         <v>185</v>
       </c>
-      <c r="C71" s="203"/>
-      <c r="D71" s="204"/>
-      <c r="E71" s="205"/>
-      <c r="F71" s="205"/>
-      <c r="G71" s="205"/>
-      <c r="H71" s="205"/>
-      <c r="I71" s="206"/>
+      <c r="C71" s="125"/>
+      <c r="D71" s="126"/>
+      <c r="E71" s="127"/>
+      <c r="F71" s="127"/>
+      <c r="G71" s="127"/>
+      <c r="H71" s="127"/>
+      <c r="I71" s="128"/>
     </row>
     <row r="72" spans="2:9">
-      <c r="B72" s="202" t="s">
+      <c r="B72" s="124" t="s">
         <v>184</v>
       </c>
-      <c r="C72" s="203"/>
-      <c r="D72" s="204"/>
-      <c r="E72" s="205"/>
-      <c r="F72" s="205"/>
-      <c r="G72" s="205"/>
-      <c r="H72" s="205"/>
-      <c r="I72" s="206"/>
+      <c r="C72" s="125"/>
+      <c r="D72" s="126"/>
+      <c r="E72" s="127"/>
+      <c r="F72" s="127"/>
+      <c r="G72" s="127"/>
+      <c r="H72" s="127"/>
+      <c r="I72" s="128"/>
     </row>
     <row r="73" spans="2:9">
-      <c r="B73" s="202" t="s">
+      <c r="B73" s="124" t="s">
         <v>183</v>
       </c>
-      <c r="C73" s="203"/>
-      <c r="D73" s="204"/>
-      <c r="E73" s="205"/>
-      <c r="F73" s="205"/>
-      <c r="G73" s="205"/>
-      <c r="H73" s="205"/>
-      <c r="I73" s="206"/>
+      <c r="C73" s="125"/>
+      <c r="D73" s="126"/>
+      <c r="E73" s="127"/>
+      <c r="F73" s="127"/>
+      <c r="G73" s="127"/>
+      <c r="H73" s="127"/>
+      <c r="I73" s="128"/>
     </row>
     <row r="74" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B74" s="211"/>
-      <c r="C74" s="212"/>
-      <c r="D74" s="213"/>
-      <c r="E74" s="214"/>
-      <c r="F74" s="212"/>
-      <c r="G74" s="212"/>
-      <c r="H74" s="212"/>
-      <c r="I74" s="215"/>
+      <c r="B74" s="169"/>
+      <c r="C74" s="170"/>
+      <c r="D74" s="171"/>
+      <c r="E74" s="172"/>
+      <c r="F74" s="170"/>
+      <c r="G74" s="170"/>
+      <c r="H74" s="170"/>
+      <c r="I74" s="173"/>
     </row>
     <row r="75" spans="2:9" ht="15" thickBot="1">
-      <c r="B75" s="207"/>
-      <c r="C75" s="207"/>
-      <c r="D75" s="207"/>
-      <c r="E75" s="153"/>
-      <c r="F75" s="153"/>
-      <c r="G75" s="153"/>
-      <c r="H75" s="153"/>
-      <c r="I75" s="153"/>
+      <c r="B75" s="164"/>
+      <c r="C75" s="164"/>
+      <c r="D75" s="164"/>
+      <c r="E75" s="165"/>
+      <c r="F75" s="165"/>
+      <c r="G75" s="165"/>
+      <c r="H75" s="165"/>
+      <c r="I75" s="165"/>
     </row>
     <row r="76" spans="2:9" ht="15">
       <c r="B76" s="16" t="s">
@@ -4926,162 +4926,162 @@
       <c r="I76" s="18"/>
     </row>
     <row r="77" spans="2:9">
-      <c r="B77" s="190" t="s">
+      <c r="B77" s="152" t="s">
         <v>36</v>
       </c>
-      <c r="C77" s="191"/>
-      <c r="D77" s="191"/>
-      <c r="E77" s="191"/>
-      <c r="F77" s="191"/>
-      <c r="G77" s="191"/>
-      <c r="H77" s="191"/>
-      <c r="I77" s="192"/>
+      <c r="C77" s="153"/>
+      <c r="D77" s="153"/>
+      <c r="E77" s="153"/>
+      <c r="F77" s="153"/>
+      <c r="G77" s="153"/>
+      <c r="H77" s="153"/>
+      <c r="I77" s="154"/>
     </row>
     <row r="78" spans="2:9" ht="21" customHeight="1">
-      <c r="B78" s="208" t="s">
+      <c r="B78" s="166" t="s">
         <v>220</v>
       </c>
-      <c r="C78" s="209"/>
-      <c r="D78" s="209"/>
-      <c r="E78" s="209"/>
-      <c r="F78" s="209"/>
-      <c r="G78" s="209"/>
-      <c r="H78" s="209"/>
-      <c r="I78" s="210"/>
+      <c r="C78" s="167"/>
+      <c r="D78" s="167"/>
+      <c r="E78" s="167"/>
+      <c r="F78" s="167"/>
+      <c r="G78" s="167"/>
+      <c r="H78" s="167"/>
+      <c r="I78" s="168"/>
     </row>
     <row r="79" spans="2:9" ht="21" customHeight="1">
-      <c r="B79" s="208"/>
-      <c r="C79" s="209"/>
-      <c r="D79" s="209"/>
-      <c r="E79" s="209"/>
-      <c r="F79" s="209"/>
-      <c r="G79" s="209"/>
-      <c r="H79" s="209"/>
-      <c r="I79" s="210"/>
+      <c r="B79" s="166"/>
+      <c r="C79" s="167"/>
+      <c r="D79" s="167"/>
+      <c r="E79" s="167"/>
+      <c r="F79" s="167"/>
+      <c r="G79" s="167"/>
+      <c r="H79" s="167"/>
+      <c r="I79" s="168"/>
     </row>
     <row r="80" spans="2:9" ht="21" customHeight="1">
-      <c r="B80" s="208"/>
-      <c r="C80" s="209"/>
-      <c r="D80" s="209"/>
-      <c r="E80" s="209"/>
-      <c r="F80" s="209"/>
-      <c r="G80" s="209"/>
-      <c r="H80" s="209"/>
-      <c r="I80" s="210"/>
+      <c r="B80" s="166"/>
+      <c r="C80" s="167"/>
+      <c r="D80" s="167"/>
+      <c r="E80" s="167"/>
+      <c r="F80" s="167"/>
+      <c r="G80" s="167"/>
+      <c r="H80" s="167"/>
+      <c r="I80" s="168"/>
     </row>
     <row r="81" spans="2:9" ht="21" customHeight="1">
-      <c r="B81" s="208"/>
-      <c r="C81" s="209"/>
-      <c r="D81" s="209"/>
-      <c r="E81" s="209"/>
-      <c r="F81" s="209"/>
-      <c r="G81" s="209"/>
-      <c r="H81" s="209"/>
-      <c r="I81" s="210"/>
+      <c r="B81" s="166"/>
+      <c r="C81" s="167"/>
+      <c r="D81" s="167"/>
+      <c r="E81" s="167"/>
+      <c r="F81" s="167"/>
+      <c r="G81" s="167"/>
+      <c r="H81" s="167"/>
+      <c r="I81" s="168"/>
     </row>
     <row r="82" spans="2:9" ht="21" customHeight="1">
-      <c r="B82" s="208"/>
-      <c r="C82" s="209"/>
-      <c r="D82" s="209"/>
-      <c r="E82" s="209"/>
-      <c r="F82" s="209"/>
-      <c r="G82" s="209"/>
-      <c r="H82" s="209"/>
-      <c r="I82" s="210"/>
+      <c r="B82" s="166"/>
+      <c r="C82" s="167"/>
+      <c r="D82" s="167"/>
+      <c r="E82" s="167"/>
+      <c r="F82" s="167"/>
+      <c r="G82" s="167"/>
+      <c r="H82" s="167"/>
+      <c r="I82" s="168"/>
     </row>
     <row r="83" spans="2:9">
-      <c r="B83" s="190" t="s">
+      <c r="B83" s="152" t="s">
         <v>37</v>
       </c>
-      <c r="C83" s="191"/>
-      <c r="D83" s="191"/>
-      <c r="E83" s="191"/>
-      <c r="F83" s="191"/>
-      <c r="G83" s="191"/>
-      <c r="H83" s="191"/>
-      <c r="I83" s="192"/>
+      <c r="C83" s="153"/>
+      <c r="D83" s="153"/>
+      <c r="E83" s="153"/>
+      <c r="F83" s="153"/>
+      <c r="G83" s="153"/>
+      <c r="H83" s="153"/>
+      <c r="I83" s="154"/>
     </row>
     <row r="84" spans="2:9" ht="49.5" customHeight="1">
-      <c r="B84" s="196" t="s">
+      <c r="B84" s="158" t="s">
         <v>223</v>
       </c>
-      <c r="C84" s="197"/>
-      <c r="D84" s="197"/>
-      <c r="E84" s="197"/>
-      <c r="F84" s="197"/>
-      <c r="G84" s="197"/>
-      <c r="H84" s="197"/>
-      <c r="I84" s="198"/>
+      <c r="C84" s="159"/>
+      <c r="D84" s="159"/>
+      <c r="E84" s="159"/>
+      <c r="F84" s="159"/>
+      <c r="G84" s="159"/>
+      <c r="H84" s="159"/>
+      <c r="I84" s="160"/>
     </row>
     <row r="85" spans="2:9" ht="49.5" customHeight="1">
-      <c r="B85" s="196"/>
-      <c r="C85" s="197"/>
-      <c r="D85" s="197"/>
-      <c r="E85" s="197"/>
-      <c r="F85" s="197"/>
-      <c r="G85" s="197"/>
-      <c r="H85" s="197"/>
-      <c r="I85" s="198"/>
+      <c r="B85" s="158"/>
+      <c r="C85" s="159"/>
+      <c r="D85" s="159"/>
+      <c r="E85" s="159"/>
+      <c r="F85" s="159"/>
+      <c r="G85" s="159"/>
+      <c r="H85" s="159"/>
+      <c r="I85" s="160"/>
     </row>
     <row r="86" spans="2:9" ht="49.5" customHeight="1">
-      <c r="B86" s="196"/>
-      <c r="C86" s="197"/>
-      <c r="D86" s="197"/>
-      <c r="E86" s="197"/>
-      <c r="F86" s="197"/>
-      <c r="G86" s="197"/>
-      <c r="H86" s="197"/>
-      <c r="I86" s="198"/>
+      <c r="B86" s="158"/>
+      <c r="C86" s="159"/>
+      <c r="D86" s="159"/>
+      <c r="E86" s="159"/>
+      <c r="F86" s="159"/>
+      <c r="G86" s="159"/>
+      <c r="H86" s="159"/>
+      <c r="I86" s="160"/>
     </row>
     <row r="87" spans="2:9" ht="49.5" customHeight="1">
-      <c r="B87" s="196"/>
-      <c r="C87" s="197"/>
-      <c r="D87" s="197"/>
-      <c r="E87" s="197"/>
-      <c r="F87" s="197"/>
-      <c r="G87" s="197"/>
-      <c r="H87" s="197"/>
-      <c r="I87" s="198"/>
+      <c r="B87" s="158"/>
+      <c r="C87" s="159"/>
+      <c r="D87" s="159"/>
+      <c r="E87" s="159"/>
+      <c r="F87" s="159"/>
+      <c r="G87" s="159"/>
+      <c r="H87" s="159"/>
+      <c r="I87" s="160"/>
     </row>
     <row r="88" spans="2:9" ht="49.5" customHeight="1">
-      <c r="B88" s="196"/>
-      <c r="C88" s="197"/>
-      <c r="D88" s="197"/>
-      <c r="E88" s="197"/>
-      <c r="F88" s="197"/>
-      <c r="G88" s="197"/>
-      <c r="H88" s="197"/>
-      <c r="I88" s="198"/>
+      <c r="B88" s="158"/>
+      <c r="C88" s="159"/>
+      <c r="D88" s="159"/>
+      <c r="E88" s="159"/>
+      <c r="F88" s="159"/>
+      <c r="G88" s="159"/>
+      <c r="H88" s="159"/>
+      <c r="I88" s="160"/>
     </row>
     <row r="89" spans="2:9" ht="49.5" customHeight="1">
-      <c r="B89" s="196"/>
-      <c r="C89" s="197"/>
-      <c r="D89" s="197"/>
-      <c r="E89" s="197"/>
-      <c r="F89" s="197"/>
-      <c r="G89" s="197"/>
-      <c r="H89" s="197"/>
-      <c r="I89" s="198"/>
+      <c r="B89" s="158"/>
+      <c r="C89" s="159"/>
+      <c r="D89" s="159"/>
+      <c r="E89" s="159"/>
+      <c r="F89" s="159"/>
+      <c r="G89" s="159"/>
+      <c r="H89" s="159"/>
+      <c r="I89" s="160"/>
     </row>
     <row r="90" spans="2:9" ht="49.5" customHeight="1">
-      <c r="B90" s="196"/>
-      <c r="C90" s="197"/>
-      <c r="D90" s="197"/>
-      <c r="E90" s="197"/>
-      <c r="F90" s="197"/>
-      <c r="G90" s="197"/>
-      <c r="H90" s="197"/>
-      <c r="I90" s="198"/>
+      <c r="B90" s="158"/>
+      <c r="C90" s="159"/>
+      <c r="D90" s="159"/>
+      <c r="E90" s="159"/>
+      <c r="F90" s="159"/>
+      <c r="G90" s="159"/>
+      <c r="H90" s="159"/>
+      <c r="I90" s="160"/>
     </row>
     <row r="91" spans="2:9" ht="49.5" customHeight="1" thickBot="1">
-      <c r="B91" s="199"/>
-      <c r="C91" s="200"/>
-      <c r="D91" s="200"/>
-      <c r="E91" s="200"/>
-      <c r="F91" s="200"/>
-      <c r="G91" s="200"/>
-      <c r="H91" s="200"/>
-      <c r="I91" s="201"/>
+      <c r="B91" s="161"/>
+      <c r="C91" s="162"/>
+      <c r="D91" s="162"/>
+      <c r="E91" s="162"/>
+      <c r="F91" s="162"/>
+      <c r="G91" s="162"/>
+      <c r="H91" s="162"/>
+      <c r="I91" s="163"/>
     </row>
     <row r="93" spans="2:9" ht="15">
       <c r="B93" s="6" t="s">
@@ -5108,108 +5108,108 @@
       <c r="I94" s="7"/>
     </row>
     <row r="95" spans="2:9" ht="18" customHeight="1">
-      <c r="B95" s="193" t="s">
+      <c r="B95" s="155" t="s">
         <v>221</v>
       </c>
-      <c r="C95" s="194"/>
-      <c r="D95" s="194"/>
-      <c r="E95" s="194"/>
-      <c r="F95" s="194"/>
-      <c r="G95" s="194"/>
-      <c r="H95" s="194"/>
-      <c r="I95" s="195"/>
+      <c r="C95" s="156"/>
+      <c r="D95" s="156"/>
+      <c r="E95" s="156"/>
+      <c r="F95" s="156"/>
+      <c r="G95" s="156"/>
+      <c r="H95" s="156"/>
+      <c r="I95" s="157"/>
     </row>
     <row r="96" spans="2:9" ht="18" customHeight="1">
-      <c r="B96" s="196"/>
-      <c r="C96" s="197"/>
-      <c r="D96" s="197"/>
-      <c r="E96" s="197"/>
-      <c r="F96" s="197"/>
-      <c r="G96" s="197"/>
-      <c r="H96" s="197"/>
-      <c r="I96" s="198"/>
+      <c r="B96" s="158"/>
+      <c r="C96" s="159"/>
+      <c r="D96" s="159"/>
+      <c r="E96" s="159"/>
+      <c r="F96" s="159"/>
+      <c r="G96" s="159"/>
+      <c r="H96" s="159"/>
+      <c r="I96" s="160"/>
     </row>
     <row r="97" spans="2:11" ht="18" customHeight="1">
-      <c r="B97" s="196"/>
-      <c r="C97" s="197"/>
-      <c r="D97" s="197"/>
-      <c r="E97" s="197"/>
-      <c r="F97" s="197"/>
-      <c r="G97" s="197"/>
-      <c r="H97" s="197"/>
-      <c r="I97" s="198"/>
+      <c r="B97" s="158"/>
+      <c r="C97" s="159"/>
+      <c r="D97" s="159"/>
+      <c r="E97" s="159"/>
+      <c r="F97" s="159"/>
+      <c r="G97" s="159"/>
+      <c r="H97" s="159"/>
+      <c r="I97" s="160"/>
     </row>
     <row r="98" spans="2:11" ht="18" customHeight="1">
-      <c r="B98" s="196"/>
-      <c r="C98" s="197"/>
-      <c r="D98" s="197"/>
-      <c r="E98" s="197"/>
-      <c r="F98" s="197"/>
-      <c r="G98" s="197"/>
-      <c r="H98" s="197"/>
-      <c r="I98" s="198"/>
+      <c r="B98" s="158"/>
+      <c r="C98" s="159"/>
+      <c r="D98" s="159"/>
+      <c r="E98" s="159"/>
+      <c r="F98" s="159"/>
+      <c r="G98" s="159"/>
+      <c r="H98" s="159"/>
+      <c r="I98" s="160"/>
     </row>
     <row r="99" spans="2:11" ht="18" customHeight="1">
-      <c r="B99" s="196"/>
-      <c r="C99" s="197"/>
-      <c r="D99" s="197"/>
-      <c r="E99" s="197"/>
-      <c r="F99" s="197"/>
-      <c r="G99" s="197"/>
-      <c r="H99" s="197"/>
-      <c r="I99" s="198"/>
+      <c r="B99" s="158"/>
+      <c r="C99" s="159"/>
+      <c r="D99" s="159"/>
+      <c r="E99" s="159"/>
+      <c r="F99" s="159"/>
+      <c r="G99" s="159"/>
+      <c r="H99" s="159"/>
+      <c r="I99" s="160"/>
     </row>
     <row r="100" spans="2:11" ht="18" customHeight="1">
-      <c r="B100" s="196"/>
-      <c r="C100" s="197"/>
-      <c r="D100" s="197"/>
-      <c r="E100" s="197"/>
-      <c r="F100" s="197"/>
-      <c r="G100" s="197"/>
-      <c r="H100" s="197"/>
-      <c r="I100" s="198"/>
+      <c r="B100" s="158"/>
+      <c r="C100" s="159"/>
+      <c r="D100" s="159"/>
+      <c r="E100" s="159"/>
+      <c r="F100" s="159"/>
+      <c r="G100" s="159"/>
+      <c r="H100" s="159"/>
+      <c r="I100" s="160"/>
     </row>
     <row r="101" spans="2:11" ht="18" customHeight="1">
-      <c r="B101" s="196"/>
-      <c r="C101" s="197"/>
-      <c r="D101" s="197"/>
-      <c r="E101" s="197"/>
-      <c r="F101" s="197"/>
-      <c r="G101" s="197"/>
-      <c r="H101" s="197"/>
-      <c r="I101" s="198"/>
+      <c r="B101" s="158"/>
+      <c r="C101" s="159"/>
+      <c r="D101" s="159"/>
+      <c r="E101" s="159"/>
+      <c r="F101" s="159"/>
+      <c r="G101" s="159"/>
+      <c r="H101" s="159"/>
+      <c r="I101" s="160"/>
     </row>
     <row r="102" spans="2:11" ht="18" customHeight="1">
-      <c r="B102" s="196"/>
-      <c r="C102" s="197"/>
-      <c r="D102" s="197"/>
-      <c r="E102" s="197"/>
-      <c r="F102" s="197"/>
-      <c r="G102" s="197"/>
-      <c r="H102" s="197"/>
-      <c r="I102" s="198"/>
-      <c r="J102" s="135"/>
-      <c r="K102" s="136"/>
+      <c r="B102" s="158"/>
+      <c r="C102" s="159"/>
+      <c r="D102" s="159"/>
+      <c r="E102" s="159"/>
+      <c r="F102" s="159"/>
+      <c r="G102" s="159"/>
+      <c r="H102" s="159"/>
+      <c r="I102" s="160"/>
+      <c r="J102" s="213"/>
+      <c r="K102" s="214"/>
     </row>
     <row r="103" spans="2:11" ht="18" customHeight="1">
-      <c r="B103" s="196"/>
-      <c r="C103" s="197"/>
-      <c r="D103" s="197"/>
-      <c r="E103" s="197"/>
-      <c r="F103" s="197"/>
-      <c r="G103" s="197"/>
-      <c r="H103" s="197"/>
-      <c r="I103" s="198"/>
+      <c r="B103" s="158"/>
+      <c r="C103" s="159"/>
+      <c r="D103" s="159"/>
+      <c r="E103" s="159"/>
+      <c r="F103" s="159"/>
+      <c r="G103" s="159"/>
+      <c r="H103" s="159"/>
+      <c r="I103" s="160"/>
     </row>
     <row r="104" spans="2:11" ht="18" customHeight="1" thickBot="1">
-      <c r="B104" s="199"/>
-      <c r="C104" s="200"/>
-      <c r="D104" s="200"/>
-      <c r="E104" s="200"/>
-      <c r="F104" s="200"/>
-      <c r="G104" s="200"/>
-      <c r="H104" s="200"/>
-      <c r="I104" s="201"/>
+      <c r="B104" s="161"/>
+      <c r="C104" s="162"/>
+      <c r="D104" s="162"/>
+      <c r="E104" s="162"/>
+      <c r="F104" s="162"/>
+      <c r="G104" s="162"/>
+      <c r="H104" s="162"/>
+      <c r="I104" s="163"/>
     </row>
     <row r="105" spans="2:11">
       <c r="B105" s="102" t="s">
@@ -5224,11 +5224,11 @@
       <c r="I105" s="104"/>
     </row>
     <row r="106" spans="2:11" ht="171.75" customHeight="1" thickBot="1">
-      <c r="B106" s="131" t="s">
+      <c r="B106" s="197" t="s">
         <v>187</v>
       </c>
-      <c r="C106" s="132"/>
-      <c r="D106" s="132"/>
+      <c r="C106" s="198"/>
+      <c r="D106" s="198"/>
       <c r="E106" s="105"/>
       <c r="F106" s="105"/>
       <c r="G106" s="105"/>
@@ -5237,6 +5237,90 @@
     </row>
   </sheetData>
   <mergeCells count="100">
+    <mergeCell ref="C68:H68"/>
+    <mergeCell ref="B62:I62"/>
+    <mergeCell ref="C63:H63"/>
+    <mergeCell ref="C64:H64"/>
+    <mergeCell ref="C65:H65"/>
+    <mergeCell ref="C66:H66"/>
+    <mergeCell ref="C67:H67"/>
+    <mergeCell ref="B106:D106"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="J102:K102"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="B15:I21"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="D8:I8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="D10:I10"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="C55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="B83:I83"/>
+    <mergeCell ref="B95:I104"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="E73:I73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="E75:I75"/>
+    <mergeCell ref="B77:I77"/>
+    <mergeCell ref="B78:I82"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="E74:I74"/>
+    <mergeCell ref="B84:I91"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B72:D72"/>
@@ -5253,90 +5337,6 @@
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="C53:E54"/>
     <mergeCell ref="F53:F54"/>
-    <mergeCell ref="B83:I83"/>
-    <mergeCell ref="B95:I104"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="E73:I73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="E75:I75"/>
-    <mergeCell ref="B77:I77"/>
-    <mergeCell ref="B78:I82"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="E74:I74"/>
-    <mergeCell ref="B84:I91"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="C55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="D10:I10"/>
-    <mergeCell ref="C11:I11"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="B15:I21"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B25:I25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="B36:I36"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B106:D106"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="J102:K102"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="C68:H68"/>
-    <mergeCell ref="B62:I62"/>
-    <mergeCell ref="C63:H63"/>
-    <mergeCell ref="C64:H64"/>
-    <mergeCell ref="C65:H65"/>
-    <mergeCell ref="C66:H66"/>
-    <mergeCell ref="C67:H67"/>
   </mergeCells>
   <conditionalFormatting sqref="H38:H50">
     <cfRule type="colorScale" priority="3">
@@ -5373,7 +5373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -5393,7 +5393,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="37.5" customHeight="1">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="229" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="26" t="s">
@@ -5402,23 +5402,23 @@
       <c r="C1" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="232" t="s">
+      <c r="D1" s="230" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="232" t="s">
+      <c r="E1" s="230" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="232" t="s">
+      <c r="F1" s="230" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1">
-      <c r="A2" s="231"/>
+      <c r="A2" s="229"/>
       <c r="B2" s="27"/>
       <c r="C2" s="27"/>
-      <c r="D2" s="232"/>
-      <c r="E2" s="232"/>
-      <c r="F2" s="232"/>
+      <c r="D2" s="230"/>
+      <c r="E2" s="230"/>
+      <c r="F2" s="230"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="34" t="s">
@@ -5483,8 +5483,8 @@
         <f>SUM(D9*E9+D10*E10+D11*E11+D12*E12+D13*E13)</f>
         <v>51</v>
       </c>
-      <c r="G8" s="229"/>
-      <c r="H8" s="229"/>
+      <c r="G8" s="232"/>
+      <c r="H8" s="232"/>
     </row>
     <row r="9" spans="1:8" ht="15.75">
       <c r="A9" s="113" t="s">
@@ -5496,8 +5496,8 @@
       <c r="E9" s="56">
         <v>3</v>
       </c>
-      <c r="G9" s="229"/>
-      <c r="H9" s="229"/>
+      <c r="G9" s="232"/>
+      <c r="H9" s="232"/>
     </row>
     <row r="10" spans="1:8" ht="15.75">
       <c r="A10" s="114" t="s">
@@ -5509,8 +5509,8 @@
       <c r="E10" s="56">
         <v>3</v>
       </c>
-      <c r="G10" s="229"/>
-      <c r="H10" s="229"/>
+      <c r="G10" s="232"/>
+      <c r="H10" s="232"/>
     </row>
     <row r="11" spans="1:8" ht="15.75">
       <c r="A11" s="114" t="s">
@@ -5522,8 +5522,8 @@
       <c r="E11" s="56">
         <v>3</v>
       </c>
-      <c r="G11" s="229"/>
-      <c r="H11" s="229"/>
+      <c r="G11" s="232"/>
+      <c r="H11" s="232"/>
     </row>
     <row r="12" spans="1:8" ht="15.75">
       <c r="A12" s="115" t="s">
@@ -5535,8 +5535,8 @@
       <c r="E12" s="56">
         <v>3</v>
       </c>
-      <c r="G12" s="229"/>
-      <c r="H12" s="229"/>
+      <c r="G12" s="232"/>
+      <c r="H12" s="232"/>
     </row>
     <row r="13" spans="1:8" ht="15.75">
       <c r="A13" s="114" t="s">
@@ -5548,8 +5548,8 @@
       <c r="E13" s="56">
         <v>3</v>
       </c>
-      <c r="G13" s="229"/>
-      <c r="H13" s="229"/>
+      <c r="G13" s="232"/>
+      <c r="H13" s="232"/>
     </row>
     <row r="14" spans="1:8" ht="15.75">
       <c r="A14" s="34" t="s">
@@ -5563,8 +5563,8 @@
         <f>SUM(D15:D22)*3</f>
         <v>72</v>
       </c>
-      <c r="G14" s="229"/>
-      <c r="H14" s="229"/>
+      <c r="G14" s="232"/>
+      <c r="H14" s="232"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="28" t="s">
@@ -5576,8 +5576,8 @@
       <c r="E15" s="57">
         <v>3</v>
       </c>
-      <c r="G15" s="229"/>
-      <c r="H15" s="229"/>
+      <c r="G15" s="232"/>
+      <c r="H15" s="232"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -5589,8 +5589,8 @@
       <c r="E16" s="57">
         <v>3</v>
       </c>
-      <c r="G16" s="229"/>
-      <c r="H16" s="229"/>
+      <c r="G16" s="232"/>
+      <c r="H16" s="232"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
@@ -5602,8 +5602,8 @@
       <c r="E17" s="57">
         <v>3</v>
       </c>
-      <c r="G17" s="229"/>
-      <c r="H17" s="229"/>
+      <c r="G17" s="232"/>
+      <c r="H17" s="232"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="107" t="s">
@@ -5615,35 +5615,35 @@
       <c r="E18" s="57">
         <v>3</v>
       </c>
-      <c r="G18" s="229"/>
-      <c r="H18" s="229"/>
+      <c r="G18" s="232"/>
+      <c r="H18" s="232"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="107"/>
       <c r="D19" s="57"/>
       <c r="E19" s="57"/>
-      <c r="G19" s="229"/>
-      <c r="H19" s="229"/>
+      <c r="G19" s="232"/>
+      <c r="H19" s="232"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="107"/>
       <c r="D20" s="57"/>
       <c r="E20" s="57"/>
-      <c r="G20" s="229"/>
-      <c r="H20" s="229"/>
+      <c r="G20" s="232"/>
+      <c r="H20" s="232"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="107"/>
       <c r="D21" s="57"/>
       <c r="E21" s="57"/>
-      <c r="G21" s="229"/>
-      <c r="H21" s="229"/>
+      <c r="G21" s="232"/>
+      <c r="H21" s="232"/>
     </row>
     <row r="22" spans="1:11">
       <c r="D22" s="57"/>
       <c r="E22" s="57"/>
-      <c r="G22" s="229"/>
-      <c r="H22" s="229"/>
+      <c r="G22" s="232"/>
+      <c r="H22" s="232"/>
     </row>
     <row r="23" spans="1:11" ht="15.75">
       <c r="A23" s="34" t="s">
@@ -5657,8 +5657,8 @@
         <f>SUM(D24:D32)*3</f>
         <v>84</v>
       </c>
-      <c r="G23" s="229"/>
-      <c r="H23" s="229"/>
+      <c r="G23" s="232"/>
+      <c r="H23" s="232"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="28" t="s">
@@ -5956,38 +5956,38 @@
       <c r="A52" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="230" t="s">
+      <c r="D52" s="231" t="s">
         <v>61</v>
       </c>
-      <c r="E52" s="230"/>
+      <c r="E52" s="231"/>
       <c r="F52" s="41">
         <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="D53" s="230" t="s">
+      <c r="D53" s="231" t="s">
         <v>62</v>
       </c>
-      <c r="E53" s="230"/>
+      <c r="E53" s="231"/>
       <c r="F53" s="40">
         <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="D54" s="230" t="s">
+      <c r="D54" s="231" t="s">
         <v>63</v>
       </c>
-      <c r="E54" s="230"/>
+      <c r="E54" s="231"/>
       <c r="F54" s="40">
         <f>F53*F52</f>
         <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:7">
-      <c r="D55" s="230" t="s">
+      <c r="D55" s="231" t="s">
         <v>94</v>
       </c>
-      <c r="E55" s="230"/>
+      <c r="E55" s="231"/>
       <c r="F55" s="39">
         <f>D46/F54</f>
         <v>11.222222222222221</v>
@@ -5995,10 +5995,10 @@
       <c r="G55" s="37"/>
     </row>
     <row r="56" spans="1:7">
-      <c r="D56" s="230" t="s">
+      <c r="D56" s="231" t="s">
         <v>95</v>
       </c>
-      <c r="E56" s="230"/>
+      <c r="E56" s="231"/>
       <c r="F56" s="39">
         <f>D49/F54</f>
         <v>14.588888888888889</v>
@@ -6006,16 +6006,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G8:H23"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D54:E54"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G8:H23"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D54:E54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>